<commit_message>
just trying to display the data in the graphs now
</commit_message>
<xml_diff>
--- a/Prototype BackUp/PrototypeFinal/Prototype/bin/Release/Made/M/Field/MDecathlon.xlsx
+++ b/Prototype BackUp/PrototypeFinal/Prototype/bin/Release/Made/M/Field/MDecathlon.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="105" windowWidth="21015" windowHeight="10230"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
   </bookViews>
   <sheets>
     <sheet name="MDecathlon" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1564" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="92">
   <si>
     <t>.</t>
   </si>
@@ -330,7 +330,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF002288"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -349,7 +349,7 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FF002288"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -535,7 +535,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -572,15 +572,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="6" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -619,7 +610,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
+  <c:lang val="en-NZ"/>
   <c:protection>
     <c:data val="1"/>
   </c:protection>
@@ -6786,13 +6777,15 @@
             <c:order val="2"/>
           </c:trendline>
           <c:xVal>
-            <c:numRef>
+            <c:strRef>
               <c:f>MDecathlon!$K$126:$K$128</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-              </c:numCache>
-            </c:numRef>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
@@ -6800,6 +6793,9 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -7825,11 +7821,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="91574656"/>
-        <c:axId val="91576576"/>
+        <c:axId val="61421056"/>
+        <c:axId val="61422976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91574656"/>
+        <c:axId val="61421056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34"/>
@@ -7863,7 +7859,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.4908062238076662"/>
+              <c:x val="0.49080622380766692"/>
               <c:y val="0.94397352504849963"/>
             </c:manualLayout>
           </c:layout>
@@ -7902,14 +7898,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91576576"/>
+        <c:crossAx val="61422976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="91576576"/>
+        <c:axId val="61422976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9000"/>
@@ -7943,7 +7939,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="7.0724032424124353E-3"/>
+              <c:x val="7.0724032424124431E-3"/>
               <c:y val="0.41426184545522515"/>
             </c:manualLayout>
           </c:layout>
@@ -7982,7 +7978,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91574656"/>
+        <c:crossAx val="61421056"/>
         <c:crossesAt val="14"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
@@ -8032,7 +8028,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196850393659" l="0.74803149606299801" r="0.74803149606299801" t="0.98425196850393659" header="0.51181102362204722" footer="0.51181102362204722"/>
+    <c:pageMargins b="0.98425196850393659" l="0.74803149606299868" r="0.74803149606299868" t="0.98425196850393659" header="0.51181102362204722" footer="0.51181102362204722"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="-3" verticalDpi="-3"/>
   </c:printSettings>
 </c:chartSpace>
@@ -8365,8 +8361,8 @@
   </sheetPr>
   <dimension ref="A1:AL150"/>
   <sheetViews>
-    <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" topLeftCell="S1" zoomScale="85" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T1" zoomScale="85" workbookViewId="0">
+      <selection sqref="A1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
@@ -8401,66 +8397,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="D1" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="E1" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="27" t="s">
+      <c r="F1" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="27" t="s">
+      <c r="G1" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="27" t="s">
+      <c r="P1" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" s="27" t="s">
+      <c r="Q1" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="23" t="s">
         <v>74</v>
       </c>
       <c r="AH1" s="2"/>
-      <c r="AI1" s="24" t="s">
+      <c r="AI1" s="21" t="s">
         <v>73</v>
       </c>
       <c r="AJ1" s="4"/>
-      <c r="AK1" s="25" t="s">
+      <c r="AK1" s="22" t="s">
         <v>72</v>
       </c>
     </row>
@@ -8520,11 +8516,11 @@
         <v>28.01</v>
       </c>
       <c r="AH2" s="2"/>
-      <c r="AI2" s="24">
+      <c r="AI2" s="21">
         <v>38437</v>
       </c>
       <c r="AJ2" s="4"/>
-      <c r="AK2" s="23">
+      <c r="AK2" s="20">
         <f>D3</f>
         <v>8056</v>
       </c>
@@ -10498,73 +10494,73 @@
       <c r="AK34" s="7"/>
     </row>
     <row r="35" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="17">
+      <c r="C35" s="13">
         <v>22.89</v>
       </c>
-      <c r="D35" s="17">
+      <c r="D35" s="13">
         <v>8402</v>
       </c>
-      <c r="E35" s="17" t="s">
+      <c r="E35" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G35" s="17">
+      <c r="G35" s="13">
         <v>29.38</v>
       </c>
-      <c r="H35" s="17">
+      <c r="H35" s="13">
         <v>8327</v>
       </c>
-      <c r="I35" s="17" t="s">
+      <c r="I35" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J35" s="17" t="s">
+      <c r="J35" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K35" s="17">
+      <c r="K35" s="13">
         <v>23.07</v>
       </c>
-      <c r="L35" s="17">
+      <c r="L35" s="13">
         <v>7637</v>
       </c>
-      <c r="M35" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N35" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O35" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P35" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R35" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S35" s="19"/>
-      <c r="T35" s="19"/>
-      <c r="U35" s="19"/>
-      <c r="V35" s="19"/>
-      <c r="W35" s="19"/>
-      <c r="X35" s="19"/>
-      <c r="Y35" s="19"/>
-      <c r="Z35" s="19"/>
-      <c r="AA35" s="19"/>
-      <c r="AB35" s="19"/>
-      <c r="AC35" s="19"/>
-      <c r="AD35" s="19"/>
-      <c r="AE35" s="19"/>
+      <c r="M35" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N35" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O35" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P35" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R35" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="16"/>
+      <c r="Z35" s="16"/>
+      <c r="AA35" s="16"/>
+      <c r="AB35" s="16"/>
+      <c r="AC35" s="16"/>
+      <c r="AD35" s="16"/>
+      <c r="AE35" s="16"/>
       <c r="AF35" s="15"/>
       <c r="AG35" s="15"/>
       <c r="AH35" s="2"/>
@@ -10576,77 +10572,77 @@
       <c r="AK35" s="7"/>
     </row>
     <row r="36" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="17">
+      <c r="C36" s="13">
         <v>26.19</v>
       </c>
-      <c r="D36" s="17">
+      <c r="D36" s="13">
         <v>8435</v>
       </c>
-      <c r="E36" s="17" t="s">
+      <c r="E36" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G36" s="17">
+      <c r="G36" s="13">
         <v>33.39</v>
       </c>
-      <c r="H36" s="17">
+      <c r="H36" s="13">
         <v>8438</v>
       </c>
-      <c r="I36" s="17" t="s">
+      <c r="I36" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J36" s="17" t="s">
+      <c r="J36" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K36" s="17">
+      <c r="K36" s="13">
         <v>25</v>
       </c>
-      <c r="L36" s="17">
+      <c r="L36" s="13">
         <v>8015</v>
       </c>
-      <c r="M36" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N36" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O36" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P36" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q36" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R36" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S36" s="19"/>
-      <c r="T36" s="19" t="s">
+      <c r="M36" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N36" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O36" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P36" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q36" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R36" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="U36" s="19" t="s">
+      <c r="U36" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="V36" s="19"/>
-      <c r="W36" s="19"/>
-      <c r="X36" s="19"/>
-      <c r="Y36" s="19"/>
-      <c r="Z36" s="19"/>
-      <c r="AA36" s="19"/>
-      <c r="AB36" s="19"/>
-      <c r="AC36" s="19"/>
-      <c r="AD36" s="19"/>
-      <c r="AE36" s="19"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="16"/>
+      <c r="X36" s="16"/>
+      <c r="Y36" s="16"/>
+      <c r="Z36" s="16"/>
+      <c r="AA36" s="16"/>
+      <c r="AB36" s="16"/>
+      <c r="AC36" s="16"/>
+      <c r="AD36" s="16"/>
+      <c r="AE36" s="16"/>
       <c r="AF36" s="15"/>
       <c r="AG36" s="15"/>
       <c r="AH36" s="2"/>
@@ -10658,74 +10654,74 @@
       <c r="AK36" s="7"/>
     </row>
     <row r="37" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A37" s="18"/>
-      <c r="B37" s="17" t="s">
+      <c r="A37" s="14"/>
+      <c r="B37" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E37" s="17"/>
-      <c r="F37" s="17" t="s">
+      <c r="C37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I37" s="17"/>
-      <c r="J37" s="17" t="s">
+      <c r="G37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I37" s="13"/>
+      <c r="J37" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="L37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q37" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R37" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S37" s="22" t="s">
+      <c r="K37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="L37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R37" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S37" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="T37" s="21">
+      <c r="T37" s="18">
         <v>1.1284722222222223E-4</v>
       </c>
-      <c r="U37" s="20">
+      <c r="U37" s="17">
         <f>T37</f>
         <v>1.1284722222222223E-4</v>
       </c>
-      <c r="V37" s="19"/>
-      <c r="W37" s="19"/>
-      <c r="X37" s="19"/>
-      <c r="Y37" s="19"/>
-      <c r="Z37" s="19"/>
-      <c r="AA37" s="19"/>
-      <c r="AB37" s="19"/>
-      <c r="AC37" s="19"/>
-      <c r="AD37" s="19"/>
-      <c r="AE37" s="19"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="16"/>
+      <c r="X37" s="16"/>
+      <c r="Y37" s="16"/>
+      <c r="Z37" s="16"/>
+      <c r="AA37" s="16"/>
+      <c r="AB37" s="16"/>
+      <c r="AC37" s="16"/>
+      <c r="AD37" s="16"/>
+      <c r="AE37" s="16"/>
       <c r="AF37" s="15"/>
       <c r="AG37" s="15"/>
       <c r="AH37" s="2"/>
@@ -10737,80 +10733,80 @@
       <c r="AK37" s="7"/>
     </row>
     <row r="38" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C38" s="17">
+      <c r="C38" s="13">
         <v>17.54</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="13">
         <v>7112</v>
       </c>
-      <c r="E38" s="17" t="s">
+      <c r="E38" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F38" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G38" s="17">
+      <c r="G38" s="13">
         <v>19.12</v>
       </c>
-      <c r="H38" s="17">
+      <c r="H38" s="13">
         <v>6932</v>
       </c>
-      <c r="I38" s="17" t="s">
+      <c r="I38" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="J38" s="17" t="s">
+      <c r="J38" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K38" s="17">
+      <c r="K38" s="13">
         <v>19.489999999999998</v>
       </c>
-      <c r="L38" s="17">
+      <c r="L38" s="13">
         <v>7499</v>
       </c>
-      <c r="M38" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N38" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O38" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P38" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R38" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S38" s="22" t="s">
+      <c r="M38" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N38" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O38" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P38" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R38" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S38" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="T38" s="21">
+      <c r="T38" s="18">
         <v>1.273148148148148E-4</v>
       </c>
-      <c r="U38" s="20">
+      <c r="U38" s="17">
         <f>T38</f>
         <v>1.273148148148148E-4</v>
       </c>
-      <c r="V38" s="19"/>
-      <c r="W38" s="19"/>
-      <c r="X38" s="19"/>
-      <c r="Y38" s="19"/>
-      <c r="Z38" s="19"/>
-      <c r="AA38" s="19"/>
-      <c r="AB38" s="19"/>
-      <c r="AC38" s="19"/>
-      <c r="AD38" s="19"/>
-      <c r="AE38" s="19"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="16"/>
+      <c r="X38" s="16"/>
+      <c r="Y38" s="16"/>
+      <c r="Z38" s="16"/>
+      <c r="AA38" s="16"/>
+      <c r="AB38" s="16"/>
+      <c r="AC38" s="16"/>
+      <c r="AD38" s="16"/>
+      <c r="AE38" s="16"/>
       <c r="AF38" s="15"/>
       <c r="AG38" s="15"/>
       <c r="AH38" s="2"/>
@@ -10822,80 +10818,80 @@
       <c r="AK38" s="7"/>
     </row>
     <row r="39" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A39" s="18" t="s">
+      <c r="A39" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C39" s="17">
+      <c r="C39" s="13">
         <v>19.75</v>
       </c>
-      <c r="D39" s="17">
+      <c r="D39" s="13">
         <v>7937</v>
       </c>
-      <c r="E39" s="17" t="s">
+      <c r="E39" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F39" s="17" t="s">
+      <c r="F39" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G39" s="17">
+      <c r="G39" s="13">
         <v>21.73</v>
       </c>
-      <c r="H39" s="17">
+      <c r="H39" s="13">
         <v>7618</v>
       </c>
-      <c r="I39" s="17" t="s">
+      <c r="I39" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="J39" s="17" t="s">
+      <c r="J39" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K39" s="17">
+      <c r="K39" s="13">
         <v>22.39</v>
       </c>
-      <c r="L39" s="17">
+      <c r="L39" s="13">
         <v>7822</v>
       </c>
-      <c r="M39" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N39" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O39" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P39" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R39" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S39" s="22" t="s">
+      <c r="M39" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N39" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O39" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P39" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R39" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S39" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="T39" s="21">
+      <c r="T39" s="18">
         <v>2.8935185185185184E-6</v>
       </c>
-      <c r="U39" s="20">
+      <c r="U39" s="17">
         <f>T39</f>
         <v>2.8935185185185184E-6</v>
       </c>
-      <c r="V39" s="19"/>
-      <c r="W39" s="19"/>
-      <c r="X39" s="19"/>
-      <c r="Y39" s="19"/>
-      <c r="Z39" s="19"/>
-      <c r="AA39" s="19"/>
-      <c r="AB39" s="19"/>
-      <c r="AC39" s="19"/>
-      <c r="AD39" s="19"/>
-      <c r="AE39" s="19"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="16"/>
+      <c r="Y39" s="16"/>
+      <c r="Z39" s="16"/>
+      <c r="AA39" s="16"/>
+      <c r="AB39" s="16"/>
+      <c r="AC39" s="16"/>
+      <c r="AD39" s="16"/>
+      <c r="AE39" s="16"/>
       <c r="AF39" s="15"/>
       <c r="AG39" s="15"/>
       <c r="AH39" s="2"/>
@@ -10907,80 +10903,80 @@
       <c r="AK39" s="7"/>
     </row>
     <row r="40" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C40" s="17">
+      <c r="C40" s="13">
         <v>21.97</v>
       </c>
-      <c r="D40" s="17">
+      <c r="D40" s="13">
         <v>8549</v>
       </c>
-      <c r="E40" s="17" t="s">
+      <c r="E40" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G40" s="17">
+      <c r="G40" s="13">
         <v>24.34</v>
       </c>
-      <c r="H40" s="17">
+      <c r="H40" s="13">
         <v>8159</v>
       </c>
-      <c r="I40" s="17" t="s">
+      <c r="I40" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="J40" s="17" t="s">
+      <c r="J40" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K40" s="17">
+      <c r="K40" s="13">
         <v>25.29</v>
       </c>
-      <c r="L40" s="17">
+      <c r="L40" s="13">
         <v>7837</v>
       </c>
-      <c r="M40" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N40" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O40" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P40" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R40" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S40" s="22" t="s">
+      <c r="M40" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N40" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O40" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P40" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R40" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S40" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="T40" s="21">
+      <c r="T40" s="18">
         <v>5.787037037037037E-7</v>
       </c>
-      <c r="U40" s="20">
+      <c r="U40" s="17">
         <f>T40</f>
         <v>5.787037037037037E-7</v>
       </c>
-      <c r="V40" s="19"/>
-      <c r="W40" s="19"/>
-      <c r="X40" s="19"/>
-      <c r="Y40" s="19"/>
-      <c r="Z40" s="19"/>
-      <c r="AA40" s="19"/>
-      <c r="AB40" s="19"/>
-      <c r="AC40" s="19"/>
-      <c r="AD40" s="19"/>
-      <c r="AE40" s="19"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="16"/>
+      <c r="X40" s="16"/>
+      <c r="Y40" s="16"/>
+      <c r="Z40" s="16"/>
+      <c r="AA40" s="16"/>
+      <c r="AB40" s="16"/>
+      <c r="AC40" s="16"/>
+      <c r="AD40" s="16"/>
+      <c r="AE40" s="16"/>
       <c r="AF40" s="15"/>
       <c r="AG40" s="15"/>
       <c r="AH40" s="2"/>
@@ -10992,67 +10988,67 @@
       <c r="AK40" s="7"/>
     </row>
     <row r="41" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A41" s="18"/>
-      <c r="B41" s="17" t="s">
+      <c r="A41" s="14"/>
+      <c r="B41" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E41" s="17"/>
-      <c r="F41" s="17" t="s">
+      <c r="C41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I41" s="17"/>
-      <c r="J41" s="17" t="s">
+      <c r="G41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I41" s="13"/>
+      <c r="J41" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="L41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q41" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R41" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S41" s="19"/>
-      <c r="T41" s="19"/>
-      <c r="U41" s="19"/>
-      <c r="V41" s="19"/>
-      <c r="W41" s="19"/>
-      <c r="X41" s="19"/>
-      <c r="Y41" s="19"/>
-      <c r="Z41" s="19"/>
-      <c r="AA41" s="19"/>
-      <c r="AB41" s="19"/>
-      <c r="AC41" s="19"/>
-      <c r="AD41" s="19"/>
-      <c r="AE41" s="19"/>
+      <c r="K41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R41" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S41" s="16"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="16"/>
+      <c r="W41" s="16"/>
+      <c r="X41" s="16"/>
+      <c r="Y41" s="16"/>
+      <c r="Z41" s="16"/>
+      <c r="AA41" s="16"/>
+      <c r="AB41" s="16"/>
+      <c r="AC41" s="16"/>
+      <c r="AD41" s="16"/>
+      <c r="AE41" s="16"/>
       <c r="AF41" s="15"/>
       <c r="AG41" s="15"/>
       <c r="AH41" s="2"/>
@@ -11064,73 +11060,73 @@
       <c r="AK41" s="7"/>
     </row>
     <row r="42" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C42" s="17">
+      <c r="C42" s="13">
         <v>18.77</v>
       </c>
-      <c r="D42" s="17">
+      <c r="D42" s="13">
         <v>6988</v>
       </c>
-      <c r="E42" s="17" t="s">
+      <c r="E42" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="F42" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G42" s="17">
+      <c r="G42" s="13">
         <v>20.78</v>
       </c>
-      <c r="H42" s="17">
+      <c r="H42" s="13">
         <v>7574</v>
       </c>
-      <c r="I42" s="17" t="s">
+      <c r="I42" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="J42" s="17" t="s">
+      <c r="J42" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K42" s="17">
+      <c r="K42" s="13">
         <v>20.46</v>
       </c>
-      <c r="L42" s="17">
+      <c r="L42" s="13">
         <v>6790</v>
       </c>
-      <c r="M42" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N42" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O42" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P42" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q42" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R42" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S42" s="19"/>
-      <c r="T42" s="19"/>
-      <c r="U42" s="19"/>
-      <c r="V42" s="19"/>
-      <c r="W42" s="19"/>
-      <c r="X42" s="19"/>
-      <c r="Y42" s="19"/>
-      <c r="Z42" s="19"/>
-      <c r="AA42" s="19"/>
-      <c r="AB42" s="19"/>
-      <c r="AC42" s="19"/>
-      <c r="AD42" s="19"/>
-      <c r="AE42" s="19"/>
+      <c r="M42" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N42" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O42" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P42" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R42" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="16"/>
+      <c r="V42" s="16"/>
+      <c r="W42" s="16"/>
+      <c r="X42" s="16"/>
+      <c r="Y42" s="16"/>
+      <c r="Z42" s="16"/>
+      <c r="AA42" s="16"/>
+      <c r="AB42" s="16"/>
+      <c r="AC42" s="16"/>
+      <c r="AD42" s="16"/>
+      <c r="AE42" s="16"/>
       <c r="AF42" s="15"/>
       <c r="AG42" s="15"/>
       <c r="AH42" s="2"/>
@@ -11142,73 +11138,73 @@
       <c r="AK42" s="7"/>
     </row>
     <row r="43" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A43" s="18" t="s">
+      <c r="A43" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="17">
+      <c r="C43" s="13">
         <v>23.75</v>
       </c>
-      <c r="D43" s="17">
+      <c r="D43" s="13">
         <v>7981</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E43" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="F43" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G43" s="17">
+      <c r="G43" s="13">
         <v>22.42</v>
       </c>
-      <c r="H43" s="17">
+      <c r="H43" s="13">
         <v>7959</v>
       </c>
-      <c r="I43" s="17" t="s">
+      <c r="I43" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="J43" s="17" t="s">
+      <c r="J43" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K43" s="17">
+      <c r="K43" s="13">
         <v>24.07</v>
       </c>
-      <c r="L43" s="17">
+      <c r="L43" s="13">
         <v>7466</v>
       </c>
-      <c r="M43" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N43" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O43" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P43" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q43" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R43" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S43" s="19"/>
-      <c r="T43" s="19"/>
-      <c r="U43" s="19"/>
-      <c r="V43" s="19"/>
-      <c r="W43" s="19"/>
-      <c r="X43" s="19"/>
-      <c r="Y43" s="19"/>
-      <c r="Z43" s="19"/>
-      <c r="AA43" s="19"/>
-      <c r="AB43" s="19"/>
-      <c r="AC43" s="19"/>
-      <c r="AD43" s="19"/>
-      <c r="AE43" s="19"/>
+      <c r="M43" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N43" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O43" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P43" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R43" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="16"/>
+      <c r="X43" s="16"/>
+      <c r="Y43" s="16"/>
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="16"/>
+      <c r="AC43" s="16"/>
+      <c r="AD43" s="16"/>
+      <c r="AE43" s="16"/>
       <c r="AF43" s="15"/>
       <c r="AG43" s="15"/>
       <c r="AH43" s="2"/>
@@ -11220,73 +11216,73 @@
       <c r="AK43" s="7"/>
     </row>
     <row r="44" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A44" s="18" t="s">
+      <c r="A44" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="17">
+      <c r="C44" s="13">
         <v>28.73</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="13">
         <v>8297</v>
       </c>
-      <c r="E44" s="17" t="s">
+      <c r="E44" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="F44" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G44" s="17">
+      <c r="G44" s="13">
         <v>24.07</v>
       </c>
-      <c r="H44" s="17">
+      <c r="H44" s="13">
         <v>8263</v>
       </c>
-      <c r="I44" s="17" t="s">
+      <c r="I44" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="J44" s="17" t="s">
+      <c r="J44" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K44" s="17">
+      <c r="K44" s="13">
         <v>27.68</v>
       </c>
-      <c r="L44" s="17">
+      <c r="L44" s="13">
         <v>8075</v>
       </c>
-      <c r="M44" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N44" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O44" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P44" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q44" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R44" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S44" s="19"/>
-      <c r="T44" s="19"/>
-      <c r="U44" s="19"/>
-      <c r="V44" s="19"/>
-      <c r="W44" s="19"/>
-      <c r="X44" s="19"/>
-      <c r="Y44" s="19"/>
-      <c r="Z44" s="19"/>
-      <c r="AA44" s="19"/>
-      <c r="AB44" s="19"/>
-      <c r="AC44" s="19"/>
-      <c r="AD44" s="19"/>
-      <c r="AE44" s="19"/>
+      <c r="M44" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N44" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O44" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P44" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R44" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S44" s="16"/>
+      <c r="T44" s="16"/>
+      <c r="U44" s="16"/>
+      <c r="V44" s="16"/>
+      <c r="W44" s="16"/>
+      <c r="X44" s="16"/>
+      <c r="Y44" s="16"/>
+      <c r="Z44" s="16"/>
+      <c r="AA44" s="16"/>
+      <c r="AB44" s="16"/>
+      <c r="AC44" s="16"/>
+      <c r="AD44" s="16"/>
+      <c r="AE44" s="16"/>
       <c r="AF44" s="15"/>
       <c r="AG44" s="15"/>
       <c r="AH44" s="2"/>
@@ -11298,67 +11294,67 @@
       <c r="AK44" s="7"/>
     </row>
     <row r="45" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A45" s="18"/>
-      <c r="B45" s="17" t="s">
+      <c r="A45" s="14"/>
+      <c r="B45" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E45" s="17"/>
-      <c r="F45" s="17" t="s">
+      <c r="C45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I45" s="17"/>
-      <c r="J45" s="17" t="s">
+      <c r="G45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I45" s="13"/>
+      <c r="J45" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="L45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q45" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R45" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S45" s="19"/>
-      <c r="T45" s="19"/>
-      <c r="U45" s="19"/>
-      <c r="V45" s="19"/>
-      <c r="W45" s="19"/>
-      <c r="X45" s="19"/>
-      <c r="Y45" s="19"/>
-      <c r="Z45" s="19"/>
-      <c r="AA45" s="19"/>
-      <c r="AB45" s="19"/>
-      <c r="AC45" s="19"/>
-      <c r="AD45" s="19"/>
-      <c r="AE45" s="19"/>
+      <c r="K45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="L45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q45" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R45" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S45" s="16"/>
+      <c r="T45" s="16"/>
+      <c r="U45" s="16"/>
+      <c r="V45" s="16"/>
+      <c r="W45" s="16"/>
+      <c r="X45" s="16"/>
+      <c r="Y45" s="16"/>
+      <c r="Z45" s="16"/>
+      <c r="AA45" s="16"/>
+      <c r="AB45" s="16"/>
+      <c r="AC45" s="16"/>
+      <c r="AD45" s="16"/>
+      <c r="AE45" s="16"/>
       <c r="AF45" s="15"/>
       <c r="AG45" s="15"/>
       <c r="AH45" s="2"/>
@@ -11370,73 +11366,73 @@
       <c r="AK45" s="7"/>
     </row>
     <row r="46" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A46" s="18" t="s">
+      <c r="A46" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C46" s="17">
+      <c r="C46" s="13">
         <v>21.62</v>
       </c>
-      <c r="D46" s="17">
+      <c r="D46" s="13">
         <v>8039</v>
       </c>
-      <c r="E46" s="17" t="s">
+      <c r="E46" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F46" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G46" s="17">
+      <c r="G46" s="13">
         <v>20.309999999999999</v>
       </c>
-      <c r="H46" s="17">
+      <c r="H46" s="13">
         <v>7535</v>
       </c>
-      <c r="I46" s="17" t="s">
+      <c r="I46" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J46" s="17" t="s">
+      <c r="J46" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K46" s="17">
+      <c r="K46" s="13">
         <v>17.77</v>
       </c>
-      <c r="L46" s="17">
+      <c r="L46" s="13">
         <v>7301</v>
       </c>
-      <c r="M46" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N46" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O46" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P46" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q46" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R46" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S46" s="19"/>
-      <c r="T46" s="19"/>
-      <c r="U46" s="19"/>
-      <c r="V46" s="19"/>
-      <c r="W46" s="19"/>
-      <c r="X46" s="19"/>
-      <c r="Y46" s="19"/>
-      <c r="Z46" s="19"/>
-      <c r="AA46" s="19"/>
-      <c r="AB46" s="19"/>
-      <c r="AC46" s="19"/>
-      <c r="AD46" s="19"/>
-      <c r="AE46" s="19"/>
+      <c r="M46" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N46" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O46" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P46" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R46" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S46" s="16"/>
+      <c r="T46" s="16"/>
+      <c r="U46" s="16"/>
+      <c r="V46" s="16"/>
+      <c r="W46" s="16"/>
+      <c r="X46" s="16"/>
+      <c r="Y46" s="16"/>
+      <c r="Z46" s="16"/>
+      <c r="AA46" s="16"/>
+      <c r="AB46" s="16"/>
+      <c r="AC46" s="16"/>
+      <c r="AD46" s="16"/>
+      <c r="AE46" s="16"/>
       <c r="AF46" s="15"/>
       <c r="AG46" s="15"/>
       <c r="AH46" s="2"/>
@@ -11448,73 +11444,73 @@
       <c r="AK46" s="7"/>
     </row>
     <row r="47" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C47" s="17">
+      <c r="C47" s="13">
         <v>25.84</v>
       </c>
-      <c r="D47" s="17">
+      <c r="D47" s="13">
         <v>8567</v>
       </c>
-      <c r="E47" s="17" t="s">
+      <c r="E47" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F47" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G47" s="17">
+      <c r="G47" s="13">
         <v>22.49</v>
       </c>
-      <c r="H47" s="17">
+      <c r="H47" s="13">
         <v>8020</v>
       </c>
-      <c r="I47" s="17" t="s">
+      <c r="I47" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J47" s="17" t="s">
+      <c r="J47" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K47" s="17">
+      <c r="K47" s="13">
         <v>21.57</v>
       </c>
-      <c r="L47" s="17">
+      <c r="L47" s="13">
         <v>7967</v>
       </c>
-      <c r="M47" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N47" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O47" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P47" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q47" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R47" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="S47" s="19"/>
-      <c r="T47" s="19"/>
-      <c r="U47" s="19"/>
-      <c r="V47" s="19"/>
-      <c r="W47" s="19"/>
-      <c r="X47" s="19"/>
-      <c r="Y47" s="19"/>
-      <c r="Z47" s="19"/>
-      <c r="AA47" s="19"/>
-      <c r="AB47" s="19"/>
-      <c r="AC47" s="19"/>
-      <c r="AD47" s="19"/>
-      <c r="AE47" s="19"/>
+      <c r="M47" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N47" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O47" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P47" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q47" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R47" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="S47" s="16"/>
+      <c r="T47" s="16"/>
+      <c r="U47" s="16"/>
+      <c r="V47" s="16"/>
+      <c r="W47" s="16"/>
+      <c r="X47" s="16"/>
+      <c r="Y47" s="16"/>
+      <c r="Z47" s="16"/>
+      <c r="AA47" s="16"/>
+      <c r="AB47" s="16"/>
+      <c r="AC47" s="16"/>
+      <c r="AD47" s="16"/>
+      <c r="AE47" s="16"/>
       <c r="AF47" s="15"/>
       <c r="AG47" s="15"/>
       <c r="AH47" s="2"/>
@@ -11526,58 +11522,58 @@
       <c r="AK47" s="7"/>
     </row>
     <row r="48" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C48" s="17">
+      <c r="C48" s="13">
         <v>30.06</v>
       </c>
-      <c r="D48" s="17">
+      <c r="D48" s="13">
         <v>8697</v>
       </c>
-      <c r="E48" s="17" t="s">
+      <c r="E48" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="F48" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G48" s="17">
+      <c r="G48" s="13">
         <v>24.66</v>
       </c>
-      <c r="H48" s="17">
+      <c r="H48" s="13">
         <v>8312</v>
       </c>
-      <c r="I48" s="17" t="s">
+      <c r="I48" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="J48" s="17" t="s">
+      <c r="J48" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K48" s="17">
+      <c r="K48" s="13">
         <v>25.38</v>
       </c>
-      <c r="L48" s="17">
+      <c r="L48" s="13">
         <v>8051</v>
       </c>
-      <c r="M48" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N48" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O48" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P48" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q48" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R48" s="16" t="s">
+      <c r="M48" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N48" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O48" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P48" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q48" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R48" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S48" s="15"/>
@@ -11604,52 +11600,52 @@
       <c r="AK48" s="7"/>
     </row>
     <row r="49" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A49" s="18"/>
-      <c r="B49" s="17" t="s">
+      <c r="A49" s="14"/>
+      <c r="B49" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E49" s="17"/>
-      <c r="F49" s="17" t="s">
+      <c r="C49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I49" s="17"/>
-      <c r="J49" s="17" t="s">
+      <c r="G49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I49" s="13"/>
+      <c r="J49" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="L49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q49" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R49" s="16" t="s">
+      <c r="K49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="L49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R49" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S49" s="15"/>
@@ -11676,58 +11672,58 @@
       <c r="AK49" s="7"/>
     </row>
     <row r="50" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C50" s="17">
+      <c r="C50" s="13">
         <v>19.61</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="13">
         <v>7483</v>
       </c>
-      <c r="E50" s="17" t="s">
+      <c r="E50" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="F50" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G50" s="17">
+      <c r="G50" s="13">
         <v>15.75</v>
       </c>
-      <c r="H50" s="17">
+      <c r="H50" s="13">
         <v>7245</v>
       </c>
-      <c r="I50" s="17" t="s">
+      <c r="I50" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J50" s="17" t="s">
+      <c r="J50" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K50" s="17">
+      <c r="K50" s="13">
         <v>22.22</v>
       </c>
-      <c r="L50" s="17">
+      <c r="L50" s="13">
         <v>7763</v>
       </c>
-      <c r="M50" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N50" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O50" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P50" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q50" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R50" s="16" t="s">
+      <c r="M50" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N50" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O50" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P50" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q50" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R50" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S50" s="15"/>
@@ -11754,58 +11750,58 @@
       <c r="AK50" s="7"/>
     </row>
     <row r="51" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B51" s="17" t="s">
+      <c r="B51" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C51" s="17">
+      <c r="C51" s="13">
         <v>24.79</v>
       </c>
-      <c r="D51" s="17">
+      <c r="D51" s="13">
         <v>8435</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="E51" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G51" s="17">
+      <c r="G51" s="13">
         <v>19.78</v>
       </c>
-      <c r="H51" s="17">
+      <c r="H51" s="13">
         <v>7742</v>
       </c>
-      <c r="I51" s="17" t="s">
+      <c r="I51" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J51" s="17" t="s">
+      <c r="J51" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K51" s="17">
+      <c r="K51" s="13">
         <v>23.96</v>
       </c>
-      <c r="L51" s="17">
+      <c r="L51" s="13">
         <v>7922</v>
       </c>
-      <c r="M51" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N51" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O51" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P51" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q51" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R51" s="16" t="s">
+      <c r="M51" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N51" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O51" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P51" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q51" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R51" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S51" s="15"/>
@@ -11832,58 +11828,58 @@
       <c r="AK51" s="7"/>
     </row>
     <row r="52" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A52" s="18" t="s">
+      <c r="A52" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C52" s="17">
+      <c r="C52" s="13">
         <v>29.97</v>
       </c>
-      <c r="D52" s="17">
+      <c r="D52" s="13">
         <v>8669</v>
       </c>
-      <c r="E52" s="17" t="s">
+      <c r="E52" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="F52" s="17" t="s">
+      <c r="F52" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G52" s="17">
+      <c r="G52" s="13">
         <v>23.8</v>
       </c>
-      <c r="H52" s="17">
+      <c r="H52" s="13">
         <v>7846</v>
       </c>
-      <c r="I52" s="17" t="s">
+      <c r="I52" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J52" s="17" t="s">
+      <c r="J52" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K52" s="17">
+      <c r="K52" s="13">
         <v>25.71</v>
       </c>
-      <c r="L52" s="17">
+      <c r="L52" s="13">
         <v>7983</v>
       </c>
-      <c r="M52" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N52" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O52" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P52" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q52" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R52" s="16" t="s">
+      <c r="M52" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N52" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O52" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P52" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q52" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R52" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S52" s="15"/>
@@ -11910,52 +11906,52 @@
       <c r="AK52" s="7"/>
     </row>
     <row r="53" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A53" s="18"/>
-      <c r="B53" s="17" t="s">
+      <c r="A53" s="14"/>
+      <c r="B53" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E53" s="17"/>
-      <c r="F53" s="17" t="s">
+      <c r="C53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="H53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="I53" s="17"/>
-      <c r="J53" s="17" t="s">
+      <c r="G53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="H53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="I53" s="13"/>
+      <c r="J53" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="L53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="M53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q53" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R53" s="16" t="s">
+      <c r="K53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="L53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="M53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q53" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R53" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S53" s="15"/>
@@ -11982,58 +11978,58 @@
       <c r="AK53" s="7"/>
     </row>
     <row r="54" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C54" s="17">
+      <c r="C54" s="13">
         <v>19.239999999999998</v>
       </c>
-      <c r="D54" s="17">
+      <c r="D54" s="13">
         <v>7404</v>
       </c>
-      <c r="E54" s="17" t="s">
+      <c r="E54" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="F54" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G54" s="17">
+      <c r="G54" s="13">
         <v>19.78</v>
       </c>
-      <c r="H54" s="17">
+      <c r="H54" s="13">
         <v>7479</v>
       </c>
-      <c r="I54" s="17" t="s">
+      <c r="I54" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J54" s="17" t="s">
+      <c r="J54" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K54" s="17">
+      <c r="K54" s="13">
         <v>19.190000000000001</v>
       </c>
-      <c r="L54" s="17">
+      <c r="L54" s="13">
         <v>7454</v>
       </c>
-      <c r="M54" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N54" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O54" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P54" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q54" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R54" s="16" t="s">
+      <c r="M54" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N54" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O54" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P54" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R54" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S54" s="15"/>
@@ -12060,58 +12056,58 @@
       <c r="AK54" s="7"/>
     </row>
     <row r="55" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="17" t="s">
+      <c r="B55" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C55" s="17">
+      <c r="C55" s="13">
         <v>24.5</v>
       </c>
-      <c r="D55" s="17">
+      <c r="D55" s="13">
         <v>8407</v>
       </c>
-      <c r="E55" s="17" t="s">
+      <c r="E55" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F55" s="17" t="s">
+      <c r="F55" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="G55" s="17">
+      <c r="G55" s="13">
         <v>24.01</v>
       </c>
-      <c r="H55" s="17">
+      <c r="H55" s="13">
         <v>8052</v>
       </c>
-      <c r="I55" s="17" t="s">
+      <c r="I55" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="J55" s="17" t="s">
+      <c r="J55" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="K55" s="17">
+      <c r="K55" s="13">
         <v>20.23</v>
       </c>
-      <c r="L55" s="17">
+      <c r="L55" s="13">
         <v>7730</v>
       </c>
-      <c r="M55" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="N55" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="O55" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="P55" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q55" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="R55" s="16" t="s">
+      <c r="M55" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="N55" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="O55" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P55" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q55" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="R55" s="12" t="s">
         <v>0</v>
       </c>
       <c r="S55" s="15"/>
@@ -16005,25 +16001,49 @@
       </c>
       <c r="AK125" s="7"/>
     </row>
-    <row r="126" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A126" s="6"/>
-      <c r="B126" s="6"/>
-      <c r="C126" s="6"/>
-      <c r="D126" s="6"/>
-      <c r="E126" s="6"/>
-      <c r="F126" s="6"/>
-      <c r="G126" s="6"/>
-      <c r="H126" s="6"/>
-      <c r="I126" s="6"/>
-      <c r="J126" s="6"/>
-      <c r="K126" s="6"/>
-      <c r="L126" s="6"/>
-      <c r="M126" s="6"/>
-      <c r="N126" s="6"/>
-      <c r="O126" s="6"/>
-      <c r="P126" s="6"/>
-      <c r="Q126" s="6"/>
-      <c r="R126" s="6"/>
+    <row r="126" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1">
+      <c r="A126" s="11"/>
+      <c r="B126" s="10"/>
+      <c r="C126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E126" s="10"/>
+      <c r="F126" s="10"/>
+      <c r="G126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I126" s="10"/>
+      <c r="J126" s="10"/>
+      <c r="K126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="L126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q126" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="R126" s="9" t="s">
+        <v>0</v>
+      </c>
       <c r="AH126" s="2"/>
       <c r="AI126" s="8"/>
       <c r="AJ126" s="4" t="e">

</xml_diff>

<commit_message>
Collect Data -> Convert Data -> Add To Graph -> Test Display
</commit_message>
<xml_diff>
--- a/Prototype BackUp/PrototypeFinal/Prototype/bin/Release/Made/M/Field/MDecathlon.xlsx
+++ b/Prototype BackUp/PrototypeFinal/Prototype/bin/Release/Made/M/Field/MDecathlon.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="28755" windowHeight="12585"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="19095" windowHeight="12270"/>
   </bookViews>
   <sheets>
     <sheet name="MDecathlon" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1576" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1572" uniqueCount="92">
   <si>
     <t>.</t>
   </si>
@@ -305,7 +305,7 @@
     <numFmt numFmtId="165" formatCode="0.000000000"/>
     <numFmt numFmtId="166" formatCode="mm:ss.00"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +316,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -353,13 +354,8 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,8 +380,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor theme="8" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -484,6 +486,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="8" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -532,10 +545,10 @@
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -578,6 +591,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -587,13 +606,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -610,7 +629,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-NZ"/>
+  <c:lang val="en-US"/>
   <c:protection>
     <c:data val="1"/>
   </c:protection>
@@ -7821,11 +7840,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="61421056"/>
-        <c:axId val="61422976"/>
+        <c:axId val="88316544"/>
+        <c:axId val="88331008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="61421056"/>
+        <c:axId val="88316544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="34"/>
@@ -7859,7 +7878,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="0.49080622380766692"/>
+              <c:x val="0.49080622380766736"/>
               <c:y val="0.94397352504849963"/>
             </c:manualLayout>
           </c:layout>
@@ -7898,14 +7917,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61422976"/>
+        <c:crossAx val="88331008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="5"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61422976"/>
+        <c:axId val="88331008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="9000"/>
@@ -7939,7 +7958,7 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="7.0724032424124431E-3"/>
+              <c:x val="7.0724032424124474E-3"/>
               <c:y val="0.41426184545522515"/>
             </c:manualLayout>
           </c:layout>
@@ -7978,7 +7997,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61421056"/>
+        <c:crossAx val="88316544"/>
         <c:crossesAt val="14"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="500"/>
@@ -8028,7 +8047,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="0.98425196850393659" l="0.74803149606299868" r="0.74803149606299868" t="0.98425196850393659" header="0.51181102362204722" footer="0.51181102362204722"/>
+    <c:pageMargins b="0.98425196850393659" l="0.74803149606299901" r="0.74803149606299901" t="0.98425196850393659" header="0.51181102362204722" footer="0.51181102362204722"/>
     <c:pageSetup paperSize="9" orientation="landscape" horizontalDpi="-3" verticalDpi="-3"/>
   </c:printSettings>
 </c:chartSpace>
@@ -8361,29 +8380,29 @@
   </sheetPr>
   <dimension ref="A1:AL150"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="T1" zoomScale="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" workbookViewId="0">
       <selection sqref="A1:R1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="20.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="6" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="7.140625" style="6" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" style="6" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.28515625" style="6" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="7.140625" style="6" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7109375" style="6" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="6" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="9" style="6" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="6" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="10.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" style="6" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="10.5703125" style="6" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="12" style="6" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="15.5703125" style="6" hidden="1" customWidth="1"/>
-    <col min="17" max="18" width="16.28515625" style="6" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="20.28515625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="9" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="8.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" style="6" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" style="6" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9" style="6" customWidth="1"/>
+    <col min="11" max="11" width="7.140625" style="6" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" style="6" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" style="6" customWidth="1"/>
+    <col min="14" max="14" width="10.5703125" style="6" customWidth="1"/>
+    <col min="15" max="15" width="12" style="6" customWidth="1"/>
+    <col min="16" max="16" width="15.5703125" style="6" customWidth="1"/>
+    <col min="17" max="18" width="16.28515625" style="6" customWidth="1"/>
     <col min="19" max="19" width="7.85546875" style="1" customWidth="1"/>
     <col min="20" max="20" width="11.7109375" style="1" customWidth="1"/>
     <col min="21" max="21" width="15.42578125" style="1" customWidth="1"/>
@@ -8397,66 +8416,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:37" s="1" customFormat="1" ht="15" customHeight="1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="H1" s="24" t="s">
+      <c r="H1" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="I1" s="24" t="s">
+      <c r="I1" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="24" t="s">
+      <c r="J1" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="26" t="s">
         <v>80</v>
       </c>
-      <c r="M1" s="24" t="s">
+      <c r="M1" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="N1" s="24" t="s">
+      <c r="N1" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="O1" s="24" t="s">
+      <c r="O1" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="24" t="s">
+      <c r="P1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" s="24" t="s">
+      <c r="Q1" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="R1" s="23" t="s">
+      <c r="R1" s="25" t="s">
         <v>74</v>
       </c>
       <c r="AH1" s="2"/>
-      <c r="AI1" s="21" t="s">
+      <c r="AI1" s="23" t="s">
         <v>73</v>
       </c>
       <c r="AJ1" s="4"/>
-      <c r="AK1" s="22" t="s">
+      <c r="AK1" s="24" t="s">
         <v>72</v>
       </c>
     </row>
@@ -8516,11 +8535,11 @@
         <v>28.01</v>
       </c>
       <c r="AH2" s="2"/>
-      <c r="AI2" s="21">
+      <c r="AI2" s="23">
         <v>38437</v>
       </c>
       <c r="AJ2" s="4"/>
-      <c r="AK2" s="20">
+      <c r="AK2" s="22">
         <f>D3</f>
         <v>8056</v>
       </c>
@@ -8745,17 +8764,17 @@
       <c r="L6" s="13">
         <v>7260</v>
       </c>
-      <c r="M6" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="N6" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="O6" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="P6" s="13" t="s">
-        <v>0</v>
+      <c r="M6" s="20">
+        <v>8900</v>
+      </c>
+      <c r="N6" s="21">
+        <v>5350</v>
+      </c>
+      <c r="O6" s="20">
+        <v>500</v>
+      </c>
+      <c r="P6" s="20">
+        <v>100</v>
       </c>
       <c r="Q6" s="13" t="s">
         <v>0</v>
@@ -16283,7 +16302,6 @@
       <c r="AK150" s="7"/>
     </row>
   </sheetData>
-  <sheetProtection password="E455" sheet="1" scenarios="1"/>
   <autoFilter ref="A1:L122"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>